<commit_message>
worked upload to submission to database
</commit_message>
<xml_diff>
--- a/src/uploaded-files/data.xlsx
+++ b/src/uploaded-files/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mavi\Desktop\Express.js\spreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mavi\Desktop\Express.js\spreadsheet\src\uploaded-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE076E64-B00E-46FB-84E9-A3E10B2D95E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E034AF9-FDCF-43FE-AF02-5490425D5363}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,16 +33,16 @@
     <t>score</t>
   </si>
   <si>
-    <t>Praise</t>
-  </si>
-  <si>
-    <t>Mavi</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
     <t>paidFees</t>
+  </si>
+  <si>
+    <t>Loveth</t>
+  </si>
+  <si>
+    <t>Excel</t>
   </si>
 </sst>
 </file>
@@ -50,8 +50,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="170" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -90,8 +90,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,7 +375,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,32 +391,32 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2">
         <v>38057</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2">
         <v>37692</v>

</xml_diff>